<commit_message>
debug | translate merged cells and formats in xlsx to docx
</commit_message>
<xml_diff>
--- a/test/samples/sample_content_1_tbl.xlsx
+++ b/test/samples/sample_content_1_tbl.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User\Documents\Bob\Coding\Automation\end-word\test\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69468BA0-9B28-4C74-916C-6FCB674BC21F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C095C3-CC1C-490B-B503-A4944837DF46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20780" yWindow="6490" windowWidth="14900" windowHeight="9000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="returns" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -121,7 +121,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,6 +173,13 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -222,48 +232,46 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -272,8 +280,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -555,281 +570,278 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:H12"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="7.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="10.453125" customWidth="1"/>
+    <col min="9" max="9" width="14.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
     </row>
     <row r="2" spans="1:8" ht="41" x14ac:dyDescent="0.35">
-      <c r="A2" s="12"/>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="15">
         <v>4.53</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="15">
         <v>11.54</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="15">
         <v>6.63</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="15">
         <v>6.9</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="15">
         <v>7.02</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="15">
         <v>6.56</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="15">
         <v>10.1</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="15">
         <v>2.27</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="15">
         <v>5.77</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="15">
         <v>3.32</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="15">
         <v>3.45</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="15">
         <v>3.51</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="15">
         <v>3.28</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="15">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="16">
         <f>+ROUND(B3-B4,2)</f>
         <v>2.2599999999999998</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="16">
         <f t="shared" ref="C5:H5" si="0">+ROUND(C3-C4,2)</f>
         <v>5.77</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="16">
         <f t="shared" si="0"/>
         <v>3.31</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="16">
         <f t="shared" si="0"/>
         <v>3.45</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="16">
         <f t="shared" si="0"/>
         <v>3.51</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="16">
         <f t="shared" si="0"/>
         <v>3.28</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="16">
         <f t="shared" si="0"/>
         <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2" t="s">
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="9"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="10"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
     </row>
     <row r="9" spans="1:8" ht="41" x14ac:dyDescent="0.35">
-      <c r="A9" s="13"/>
-      <c r="B9" s="1" t="s">
+      <c r="A9" s="11"/>
+      <c r="B9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="15">
         <v>17.82</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="15">
         <v>44.96</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="15">
         <v>25.38</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="15">
         <v>26.4</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="15">
         <v>26.84</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="15">
         <v>25.02</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="15">
         <v>30.1</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="15">
         <v>17.739999999999998</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="15">
         <v>42.44</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="15">
         <v>20.3</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="15">
         <v>22.68</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="15">
         <v>24.8</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="15">
         <v>23.66</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="15">
         <v>23.25</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="16">
         <f t="shared" ref="B12:H12" si="1">+ROUND(B10-B11,2)</f>
         <v>0.08</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="16">
         <f t="shared" si="1"/>
         <v>2.52</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="16">
         <f t="shared" si="1"/>
         <v>5.08</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="16">
         <f t="shared" si="1"/>
         <v>3.72</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="16">
         <f t="shared" si="1"/>
         <v>2.04</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="16">
         <f t="shared" si="1"/>
         <v>1.36</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="16">
         <f t="shared" si="1"/>
         <v>6.85</v>
       </c>

</xml_diff>

<commit_message>
feature | reflect xls superscripts in docx
</commit_message>
<xml_diff>
--- a/test/samples/sample_content_1_tbl.xlsx
+++ b/test/samples/sample_content_1_tbl.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User\Documents\Bob\Coding\Automation\end-word\test\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C095C3-CC1C-490B-B503-A4944837DF46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B25BFA6-A203-4A15-B369-58F1464084C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
   <si>
     <t>Portfolio</t>
   </si>
@@ -115,6 +115,112 @@
   </si>
   <si>
     <t>Period Ending 30 September 2010 – Net** Returns</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">* Returns are expressed before deducting investment management fees.
+** Returns are expressed after deducting investment management fees.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>#</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 08 March 2007.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> From 1 January 2010, the portfolio transitioned to a predominantly global REIT strategy with the benchmark amended from the S&amp;P/ASX 300 (GICS) Property Accumulation index to the FTSE EPRA/NAREIT Developed Index (hedged in AUD).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>^</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> From 1 July 2011 the benchmark is an equally weighted composite of the hedged and unhedged FTSE EPRA/NAREIT Developed Index.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>~</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> From 1 September 2013, the benchmark is FTSE EPRA/NAREIT Developed Index (hedged in AUD).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> From 1 September 2017, the benchmark is FTSE EPRA/NAREIT Developed Index (unhedged in AUD) Net TRI.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -124,7 +230,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,6 +287,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -236,7 +355,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -274,17 +393,23 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -567,10 +692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -581,16 +706,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
     </row>
     <row r="2" spans="1:8" ht="41" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
@@ -620,25 +745,25 @@
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="13">
         <v>4.53</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="13">
         <v>11.54</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="13">
         <v>6.63</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="13">
         <v>6.9</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F3" s="13">
         <v>7.02</v>
       </c>
-      <c r="G3" s="15">
+      <c r="G3" s="13">
         <v>6.56</v>
       </c>
-      <c r="H3" s="15">
+      <c r="H3" s="13">
         <v>10.1</v>
       </c>
     </row>
@@ -646,25 +771,25 @@
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="13">
         <v>2.27</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="13">
         <v>5.77</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="13">
         <v>3.32</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="13">
         <v>3.45</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="13">
         <v>3.51</v>
       </c>
-      <c r="G4" s="15">
+      <c r="G4" s="13">
         <v>3.28</v>
       </c>
-      <c r="H4" s="15">
+      <c r="H4" s="13">
         <v>5</v>
       </c>
     </row>
@@ -672,32 +797,25 @@
       <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="16">
-        <f>+ROUND(B3-B4,2)</f>
-        <v>2.2599999999999998</v>
-      </c>
-      <c r="C5" s="16">
-        <f t="shared" ref="C5:H5" si="0">+ROUND(C3-C4,2)</f>
+      <c r="B5" s="14">
+        <v>2.2600000000000002</v>
+      </c>
+      <c r="C5" s="14">
         <v>5.77</v>
       </c>
-      <c r="D5" s="16">
-        <f t="shared" si="0"/>
+      <c r="D5" s="14">
         <v>3.31</v>
       </c>
-      <c r="E5" s="16">
-        <f t="shared" si="0"/>
+      <c r="E5" s="14">
         <v>3.45</v>
       </c>
-      <c r="F5" s="16">
-        <f t="shared" si="0"/>
+      <c r="F5" s="14">
         <v>3.51</v>
       </c>
-      <c r="G5" s="16">
-        <f t="shared" si="0"/>
+      <c r="G5" s="14">
         <v>3.28</v>
       </c>
-      <c r="H5" s="16">
-        <f t="shared" si="0"/>
+      <c r="H5" s="14">
         <v>5.0999999999999996</v>
       </c>
     </row>
@@ -726,16 +844,16 @@
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
     </row>
     <row r="9" spans="1:8" ht="41" x14ac:dyDescent="0.35">
       <c r="A9" s="11"/>
@@ -765,25 +883,25 @@
       <c r="A10" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="13">
         <v>17.82</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="13">
         <v>44.96</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="13">
         <v>25.38</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="13">
         <v>26.4</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F10" s="13">
         <v>26.84</v>
       </c>
-      <c r="G10" s="15">
+      <c r="G10" s="13">
         <v>25.02</v>
       </c>
-      <c r="H10" s="15">
+      <c r="H10" s="13">
         <v>30.1</v>
       </c>
     </row>
@@ -791,25 +909,25 @@
       <c r="A11" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="13">
         <v>17.739999999999998</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="13">
         <v>42.44</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="13">
         <v>20.3</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="13">
         <v>22.68</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="13">
         <v>24.8</v>
       </c>
-      <c r="G11" s="15">
+      <c r="G11" s="13">
         <v>23.66</v>
       </c>
-      <c r="H11" s="15">
+      <c r="H11" s="13">
         <v>23.25</v>
       </c>
     </row>
@@ -817,39 +935,45 @@
       <c r="A12" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="16">
-        <f t="shared" ref="B12:H12" si="1">+ROUND(B10-B11,2)</f>
-        <v>0.08</v>
-      </c>
-      <c r="C12" s="16">
-        <f t="shared" si="1"/>
-        <v>2.52</v>
-      </c>
-      <c r="D12" s="16">
-        <f t="shared" si="1"/>
-        <v>5.08</v>
-      </c>
-      <c r="E12" s="16">
-        <f t="shared" si="1"/>
-        <v>3.72</v>
-      </c>
-      <c r="F12" s="16">
-        <f t="shared" si="1"/>
-        <v>2.04</v>
-      </c>
-      <c r="G12" s="16">
-        <f t="shared" si="1"/>
-        <v>1.36</v>
-      </c>
-      <c r="H12" s="16">
-        <f t="shared" si="1"/>
-        <v>6.85</v>
-      </c>
+      <c r="B12" s="14">
+        <v>8.0000000000001847E-2</v>
+      </c>
+      <c r="C12" s="14">
+        <v>2.5200000000000031</v>
+      </c>
+      <c r="D12" s="14">
+        <v>5.0799999999999983</v>
+      </c>
+      <c r="E12" s="14">
+        <v>3.7199999999999989</v>
+      </c>
+      <c r="F12" s="14">
+        <v>2.0399999999999991</v>
+      </c>
+      <c r="G12" s="14">
+        <v>1.3599999999999994</v>
+      </c>
+      <c r="H12" s="14">
+        <v>6.8500000000000014</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="113" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A13:H13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add functionality to copy xls font name and size
</commit_message>
<xml_diff>
--- a/test/samples/sample_content_1_tbl.xlsx
+++ b/test/samples/sample_content_1_tbl.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User\Documents\Bob\Coding\Automation\end-word\test\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B25BFA6-A203-4A15-B369-58F1464084C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD17D73-6196-4964-A011-9AA4A6914DC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8330" yWindow="5490" windowWidth="15440" windowHeight="11880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="returns" sheetId="1" r:id="rId1"/>
@@ -117,110 +117,13 @@
     <t>Period Ending 30 September 2010 – Net** Returns</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">* Returns are expressed before deducting investment management fees.
+    <t>* Returns are expressed before deducting investment management fees.
 ** Returns are expressed after deducting investment management fees.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>#</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> 08 March 2007.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>+</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> From 1 January 2010, the portfolio transitioned to a predominantly global REIT strategy with the benchmark amended from the S&amp;P/ASX 300 (GICS) Property Accumulation index to the FTSE EPRA/NAREIT Developed Index (hedged in AUD).
-</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>^</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> From 1 July 2011 the benchmark is an equally weighted composite of the hedged and unhedged FTSE EPRA/NAREIT Developed Index.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>~</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> From 1 September 2013, the benchmark is FTSE EPRA/NAREIT Developed Index (hedged in AUD).
-</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> From 1 September 2017, the benchmark is FTSE EPRA/NAREIT Developed Index (unhedged in AUD) Net TRI.</t>
-    </r>
+# 08 March 2007.
++ From 1 January 2010, the portfolio transitioned to a predominantly global REIT strategy with the benchmark amended from the S&amp;P/ASX 300 (GICS) Property Accumulation index to the FTSE EPRA/NAREIT Developed Index (hedged in AUD).
+^ From 1 July 2011 the benchmark is an equally weighted composite of the hedged and unhedged FTSE EPRA/NAREIT Developed Index.
+~ From 1 September 2013, the benchmark is FTSE EPRA/NAREIT Developed Index (hedged in AUD).
+&gt; From 1 September 2017, the benchmark is FTSE EPRA/NAREIT Developed Index (unhedged in AUD) Net TRI.</t>
   </si>
 </sst>
 </file>
@@ -230,7 +133,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -288,15 +191,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <vertAlign val="superscript"/>
       <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -399,17 +295,17 @@
     <xf numFmtId="43" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -695,7 +591,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A13" sqref="A13:H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -706,16 +602,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
     </row>
     <row r="2" spans="1:8" ht="41" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
@@ -844,16 +740,16 @@
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
     </row>
     <row r="9" spans="1:8" ht="41" x14ac:dyDescent="0.35">
       <c r="A9" s="11"/>
@@ -957,17 +853,17 @@
         <v>6.8500000000000014</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="113" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="18" t="s">
+    <row r="13" spans="1:8" ht="101" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>